<commit_message>
tg: sch-sth oct 2021 - updates forms
</commit_message>
<xml_diff>
--- a/SCH-STH/Impact assessments/Togo/tg_sch_sth_impact_2_child_202110.xlsx
+++ b/SCH-STH/Impact assessments/Togo/tg_sch_sth_impact_2_child_202110.xlsx
@@ -1,28 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24430"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\WHO\dsa-forms\SCH-STH\Impact assessments\Togo\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05383ED7-1F80-4815-80E1-B056D1D95B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="28800" windowHeight="12345" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
     <sheet name="choices" sheetId="2" r:id="rId2"/>
     <sheet name="settings" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525" iterateDelta="1E-4"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="205">
   <si>
     <t>type</t>
   </si>
@@ -119,7 +113,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t>Select the Sub-district (</t>
     </r>
@@ -128,7 +122,7 @@
         <sz val="11"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t>USP</t>
     </r>
@@ -137,19 +131,13 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t>)</t>
     </r>
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
       <t>Sélectionner le sous-district (</t>
     </r>
     <r>
@@ -157,7 +145,7 @@
         <sz val="11"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>USP</t>
     </r>
@@ -166,7 +154,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>)</t>
     </r>
@@ -178,7 +166,7 @@
     <t>Select the site name</t>
   </si>
   <si>
-    <t>Entrez le nom de l'école</t>
+    <t>Sélectionner le nom de l'école</t>
   </si>
   <si>
     <t>p_site_id</t>
@@ -187,7 +175,7 @@
     <t>Select the site code</t>
   </si>
   <si>
-    <t>Entrez le code de l'école</t>
+    <t>Sélectionner le code de l'école</t>
   </si>
   <si>
     <t>regex(.,'^[0-9]{3}$')</t>
@@ -241,7 +229,7 @@
     <t>Comment est-ce que l'identifiant individuel sera-t-il généré?</t>
   </si>
   <si>
-    <t>${p_consent} = 'Given'</t>
+    <t>${p_consent} = 'A.donne'</t>
   </si>
   <si>
     <t>barcode</t>
@@ -250,13 +238,13 @@
     <t>p_barcodeid</t>
   </si>
   <si>
-    <t>Scan barcode now</t>
-  </si>
-  <si>
-    <t>Scanner le barcode</t>
-  </si>
-  <si>
-    <t>${p_idmethod} = 'Scanner' and ${p_consent} = 'Given'</t>
+    <t>Scan QR code now</t>
+  </si>
+  <si>
+    <t>Scanner le QR Code</t>
+  </si>
+  <si>
+    <t>${p_idmethod} = 'Scanner' and ${p_consent} = 'A.donne'</t>
   </si>
   <si>
     <t>p_code_id</t>
@@ -268,7 +256,7 @@
     <t>Veuillez enregistrer le code d'identification unique suivant pour le répondant sur une liste séparée et sur chaque test de diagnostic administré, y compris les tests Kato Katz et de Filtration Urinaire</t>
   </si>
   <si>
-    <t>${p_idmethod} != 'Scanner' and ${p_consent} = 'Given'</t>
+    <t>${p_idmethod} != 'Scanner' and ${p_consent} = 'A.donne'</t>
   </si>
   <si>
     <t>p_age_yrs</t>
@@ -306,7 +294,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t xml:space="preserve">select_one </t>
     </r>
@@ -315,7 +303,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t>yesNo</t>
     </r>
@@ -345,121 +333,28 @@
     <t>Un échantillon d’urine a-t-il été prélevé de cette personne?</t>
   </si>
   <si>
-    <t>select_one toilet_place</t>
-  </si>
-  <si>
-    <t>p_urinate_place</t>
-  </si>
-  <si>
-    <t>When you are at school, where do you usually go to urinate?</t>
-  </si>
-  <si>
-    <t>Où allez-vous habituellement pour uriner lorsque vous êtes à l'école?</t>
-  </si>
-  <si>
-    <t>${p_consent} = 'Given' and ${p_collected_stool} = 'Yes' and ${p_collected_urine} = 'Yes'</t>
-  </si>
-  <si>
-    <t>p_urinate_place_other</t>
-  </si>
-  <si>
-    <t>Please, specify other urinate place</t>
-  </si>
-  <si>
-    <t>Veuillez précisez les autres place d'urinage</t>
-  </si>
-  <si>
-    <t>${p_urinate_place} = 'Other' and ${p_consent} = 'Given' and ${p_collected_stool} = 'Yes' and ${p_collected_urine} = 'Yes'</t>
-  </si>
-  <si>
-    <t>select_one wash_hand</t>
-  </si>
-  <si>
-    <t>p_urinate_wash</t>
-  </si>
-  <si>
-    <t>Do you wash your hands after urinating?</t>
-  </si>
-  <si>
-    <t>Est-ce que vous vous lavez les mains après avoir uriner?</t>
-  </si>
-  <si>
-    <t>select_one not_was_hand_reason</t>
-  </si>
-  <si>
-    <t>p_urinate_wash_noreason</t>
-  </si>
-  <si>
-    <t>If no, why don't you wash your hand after urinating</t>
-  </si>
-  <si>
-    <t>Si non, pourquoi est-ce que vous ne vous lavez pas les mains après avoir uriner?</t>
-  </si>
-  <si>
-    <t>${p_urinate_wash} = 'No' and ${p_consent} = 'Given' and ${p_collected_stool} = 'Yes' and ${p_collected_urine} = 'Yes'</t>
-  </si>
-  <si>
-    <t>p_defecate_place</t>
-  </si>
-  <si>
-    <t>When you are at school, where do you usually go to defecate?</t>
-  </si>
-  <si>
-    <t>Où allez-vous habituellement pour déféquer lorsque vous êtes à l'école?</t>
-  </si>
-  <si>
-    <t>p_defecate_place_other</t>
-  </si>
-  <si>
-    <t>Please, specify other defecation place</t>
-  </si>
-  <si>
-    <t>Veuillez précisez les autres place de défécage</t>
-  </si>
-  <si>
-    <t>${p_defecate_place} = 'Other' and ${p_consent} = 'Given' and ${p_collected_stool} = 'Yes' and ${p_collected_urine} = 'Yes'</t>
-  </si>
-  <si>
-    <t>p_defecate_wash</t>
-  </si>
-  <si>
-    <t>Do you wash your hands after defecating?</t>
-  </si>
-  <si>
-    <t>${p_consent} = 'Given' and ${p_consent} = 'Given' and ${p_collected_stool} = 'Yes' and ${p_collected_urine} = 'Yes'</t>
-  </si>
-  <si>
-    <t>p_defecate_wash_noreason</t>
-  </si>
-  <si>
-    <t>If no, why don't you wash your hand after defecating</t>
-  </si>
-  <si>
-    <t>Est-ce que vous vous lavez les mains après avoir déféquer?</t>
-  </si>
-  <si>
-    <t>${p_defecate_wash} = 'No' and ${p_consent} = 'Given' and ${p_collected_stool} = 'Yes' and ${p_collected_urine} = 'Yes'</t>
-  </si>
-  <si>
-    <t>select_one water_activity</t>
-  </si>
-  <si>
-    <t>p_water_activities</t>
-  </si>
-  <si>
-    <t>Do you perform any of the following activities in fresh water bodies nearby?</t>
-  </si>
-  <si>
-    <t>If there are water bodies (river, stream, canal, lake, dam etc)</t>
-  </si>
-  <si>
-    <t>Laquelle des activités suivantes effectuez-vous?</t>
-  </si>
-  <si>
-    <t>S'il y a des cours d'eau (rivière, ruisseau, canal, lac, barrage, etc.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ${p_consent} = 'Given' and ${p_collected_stool} = 'Yes' and ${p_collected_urine} = 'Yes'</t>
+    <t>select_one grading</t>
+  </si>
+  <si>
+    <t>p_grading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What was the haemastix result? </t>
+  </si>
+  <si>
+    <t>Graduation de la microhématurie</t>
+  </si>
+  <si>
+    <t>${p_consent} = 'A.donne' and ${p_collected_stool} = 'Oui' and ${p_collected_urine} = 'Oui'</t>
+  </si>
+  <si>
+    <t>p_urine_conserve</t>
+  </si>
+  <si>
+    <t>Is this urine being saved for urine filtration?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cette urine est-elle conservée pour la filtration de l’urine? </t>
   </si>
   <si>
     <t>p_ending_survey_note</t>
@@ -471,7 +366,7 @@
     <t>Vous venez d'entrer une valeur qui entrainera la fin de l'enquête</t>
   </si>
   <si>
-    <t>${p_consent} = 'Refused'</t>
+    <t>${p_consent} = 'A.refuse'</t>
   </si>
   <si>
     <t>p_sample_note</t>
@@ -483,7 +378,7 @@
     <t>Vous venez d'entrer une valeur qui entrainera la fin de l'enquête. Veuillez collecter les échantillons de selle et d'urine du participant.</t>
   </si>
   <si>
-    <t>${p_collected_stool} = 'No' and ${p_collected_urine} = 'No'</t>
+    <t>${p_collected_stool} = 'Non' and ${p_collected_urine} = 'Non'</t>
   </si>
   <si>
     <t>p_remarks</t>
@@ -516,18 +411,18 @@
     <t>yesNo</t>
   </si>
   <si>
+    <t>Oui</t>
+  </si>
+  <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>Oui</t>
+    <t>Non</t>
   </si>
   <si>
     <t>No</t>
   </si>
   <si>
-    <t>Non</t>
-  </si>
-  <si>
     <t>p_IDMethod</t>
   </si>
   <si>
@@ -543,69 +438,90 @@
     <t>sex</t>
   </si>
   <si>
+    <t>Feminin</t>
+  </si>
+  <si>
     <t>Female</t>
   </si>
   <si>
     <t>Féminin</t>
   </si>
   <si>
+    <t>Masculin</t>
+  </si>
+  <si>
     <t>Male</t>
   </si>
   <si>
-    <t>Masculin</t>
-  </si>
-  <si>
     <t>toilet_place</t>
   </si>
   <si>
+    <t>Dans.les.toilettes.de.l.ecole</t>
+  </si>
+  <si>
     <t>In the school toilet</t>
   </si>
   <si>
     <t>Dans les toilettes de l'école</t>
   </si>
   <si>
+    <t>Autour.de.la.cloture.de.l.ecole</t>
+  </si>
+  <si>
     <t>Around the school compound</t>
   </si>
   <si>
     <t>Autour de la cloture de l'école</t>
   </si>
   <si>
+    <t>a.l.exterieur.de.l.ecole</t>
+  </si>
+  <si>
     <t>Outside of school compound</t>
   </si>
   <si>
     <t>À l'extérieur de l'école</t>
   </si>
   <si>
+    <t>J.attends/Je.me.retiens</t>
+  </si>
+  <si>
     <t>I wait/hold it</t>
   </si>
   <si>
     <t>J'attends/Je me retiens</t>
   </si>
   <si>
+    <t>Ne.sais.pas</t>
+  </si>
+  <si>
     <t>Don't know</t>
   </si>
   <si>
     <t>Ne sais pas</t>
   </si>
   <si>
-    <t>Other</t>
+    <t>Autres</t>
   </si>
   <si>
     <t>Others (specify)</t>
   </si>
   <si>
-    <t>Autres</t>
-  </si>
-  <si>
     <t>wash_hand</t>
   </si>
   <si>
+    <t>Oui,.avec.du.savon/cendre</t>
+  </si>
+  <si>
     <t>Yes-with soap/Ashes</t>
   </si>
   <si>
     <t>Oui, avec du savon/cendre</t>
   </si>
   <si>
+    <t>Oui,.sans.savon/cendre</t>
+  </si>
+  <si>
     <t>Yes- without soap/Ashes</t>
   </si>
   <si>
@@ -615,18 +531,27 @@
     <t>not_was_hand_reason</t>
   </si>
   <si>
+    <t>Eau.non.disponible.a.l.ecole</t>
+  </si>
+  <si>
     <t>Water not available in school</t>
   </si>
   <si>
     <t>Eau non disponible à l'école</t>
   </si>
   <si>
+    <t>J.oublie.toujours</t>
+  </si>
+  <si>
     <t>I always forget</t>
   </si>
   <si>
     <t>J'oublie toujours</t>
   </si>
   <si>
+    <t>Je.ne.pense.pas.que.ce.soit.important</t>
+  </si>
+  <si>
     <t>I don’t think it is important</t>
   </si>
   <si>
@@ -636,10 +561,13 @@
     <t>water_activity</t>
   </si>
   <si>
+    <t>Baignade</t>
+  </si>
+  <si>
     <t>Bathing</t>
   </si>
   <si>
-    <t>Baignade</t>
+    <t>Lessive,.vaisselle</t>
   </si>
   <si>
     <t>Washing clothes, dishes</t>
@@ -648,40 +576,49 @@
     <t>Lessive, vaisselle</t>
   </si>
   <si>
+    <t>Peche</t>
+  </si>
+  <si>
     <t>Fishing</t>
   </si>
   <si>
     <t>Pêche</t>
   </si>
   <si>
+    <t>Traversee.de.cours.d.eau</t>
+  </si>
+  <si>
     <t>Crossing water</t>
   </si>
   <si>
     <t>Traversée de cours d'eau</t>
   </si>
   <si>
+    <t>Puisage.de.l.eau.dans.des.cours.d.eau</t>
+  </si>
+  <si>
     <t>Fetching water</t>
   </si>
   <si>
     <t>Puisage de l'eau dans des cours d'eau</t>
   </si>
   <si>
+    <t>Jouer</t>
+  </si>
+  <si>
     <t>Playing</t>
   </si>
   <si>
-    <t>Jouer</t>
+    <t>Nager</t>
   </si>
   <si>
     <t>Swimming</t>
   </si>
   <si>
-    <t>Nager</t>
-  </si>
-  <si>
     <t>consent_list</t>
   </si>
   <si>
-    <t>Given</t>
+    <t>A.donne</t>
   </si>
   <si>
     <t>1. Given</t>
@@ -690,7 +627,7 @@
     <t>1. A donné</t>
   </si>
   <si>
-    <t>Refused</t>
+    <t>A.refuse</t>
   </si>
   <si>
     <t>2. Refused</t>
@@ -699,6 +636,45 @@
     <t>2. A refusé</t>
   </si>
   <si>
+    <t>grading</t>
+  </si>
+  <si>
+    <t>Negatif</t>
+  </si>
+  <si>
+    <t>Negative</t>
+  </si>
+  <si>
+    <t>Négatif</t>
+  </si>
+  <si>
+    <t>Trace.non.hemolysee</t>
+  </si>
+  <si>
+    <t>Trace non-haemolysed</t>
+  </si>
+  <si>
+    <t>Trace non hémolysée</t>
+  </si>
+  <si>
+    <t>Trace.hemolysee</t>
+  </si>
+  <si>
+    <t>Trace haemolysed</t>
+  </si>
+  <si>
+    <t>Trace hémolysée</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>++</t>
+  </si>
+  <si>
+    <t>+++</t>
+  </si>
+  <si>
     <t>form_title</t>
   </si>
   <si>
@@ -711,20 +687,26 @@
     <t>default_language</t>
   </si>
   <si>
-    <t>tg_sch_sth_impact_2_child_202110</t>
+    <t>(Octobre 2021) - 2. SCH/STH – Enrôlement</t>
+  </si>
+  <si>
+    <t>tg_sch_sth_impact_2_child_202110_v1_1</t>
   </si>
   <si>
     <t>French</t>
-  </si>
-  <si>
-    <t>(Octobre 2021) - 2. SCH/STH – Enrôlement</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="28">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -736,35 +718,198 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -783,8 +928,194 @@
         <bgColor rgb="FFCCFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -818,9 +1149,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -828,7 +1401,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -866,6 +1439,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -893,21 +1469,65 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" quotePrefix="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1165,87 +1785,88 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E8" activePane="bottomRight" state="frozen"/>
+      <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M13" sqref="M13:M15"/>
+      <selection pane="bottomRight" activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.7" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="19.609375" style="20" customWidth="1"/>
-    <col min="2" max="2" width="14.5" style="20" customWidth="1"/>
-    <col min="3" max="3" width="42.609375" style="20" customWidth="1"/>
-    <col min="4" max="4" width="41.21875" style="20" customWidth="1"/>
-    <col min="5" max="5" width="47.5" style="20" customWidth="1"/>
-    <col min="6" max="6" width="47.38671875" customWidth="1"/>
-    <col min="7" max="7" width="12.609375" customWidth="1"/>
-    <col min="8" max="8" width="16.88671875" customWidth="1"/>
+    <col min="1" max="1" width="19.6066666666667" style="21" customWidth="1"/>
+    <col min="2" max="2" width="14.5" style="21" customWidth="1"/>
+    <col min="3" max="3" width="42.6066666666667" style="21" customWidth="1"/>
+    <col min="4" max="4" width="41.22" style="21" customWidth="1"/>
+    <col min="5" max="5" width="47.5" style="21" customWidth="1"/>
+    <col min="6" max="6" width="47.3866666666667" customWidth="1"/>
+    <col min="7" max="7" width="12.6066666666667" customWidth="1"/>
+    <col min="8" max="8" width="16.8866666666667" customWidth="1"/>
     <col min="9" max="10" width="29.5" customWidth="1"/>
     <col min="11" max="11" width="22" customWidth="1"/>
-    <col min="12" max="12" width="12.609375" customWidth="1"/>
-    <col min="13" max="13" width="9.71875" customWidth="1"/>
-    <col min="14" max="14" width="13.88671875" customWidth="1"/>
-    <col min="15" max="15" width="36.609375" customWidth="1"/>
+    <col min="12" max="12" width="12.6066666666667" customWidth="1"/>
+    <col min="13" max="13" width="9.72" customWidth="1"/>
+    <col min="14" max="14" width="13.8866666666667" customWidth="1"/>
+    <col min="15" max="15" width="36.6066666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="3" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="21" t="s">
+    <row r="1" s="19" customFormat="1" ht="36" spans="1:15">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="K1" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="L1" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="M1" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="21" t="s">
+      <c r="N1" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="21" t="s">
+      <c r="O1" s="22" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="3" customFormat="1" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" s="19" customFormat="1" ht="31.5" spans="1:15">
       <c r="A2" s="9" t="s">
         <v>15</v>
       </c>
@@ -1282,7 +1903,7 @@
       <c r="N2" s="9"/>
       <c r="O2" s="9"/>
     </row>
-    <row r="3" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" s="19" customFormat="1" spans="1:15">
       <c r="A3" s="9" t="s">
         <v>25</v>
       </c>
@@ -1301,7 +1922,7 @@
       <c r="H3" s="16"/>
       <c r="I3" s="17"/>
       <c r="J3" s="11"/>
-      <c r="K3" s="24"/>
+      <c r="K3" s="25"/>
       <c r="L3" s="9"/>
       <c r="M3" s="9" t="s">
         <v>24</v>
@@ -1309,7 +1930,7 @@
       <c r="N3" s="9"/>
       <c r="O3" s="16"/>
     </row>
-    <row r="4" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" s="19" customFormat="1" spans="1:15">
       <c r="A4" s="9" t="s">
         <v>25</v>
       </c>
@@ -1328,7 +1949,7 @@
       <c r="H4" s="16"/>
       <c r="I4" s="17"/>
       <c r="J4" s="11"/>
-      <c r="K4" s="24"/>
+      <c r="K4" s="25"/>
       <c r="L4" s="9"/>
       <c r="M4" s="9" t="s">
         <v>24</v>
@@ -1336,7 +1957,7 @@
       <c r="N4" s="9"/>
       <c r="O4" s="16"/>
     </row>
-    <row r="5" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" s="19" customFormat="1" spans="1:15">
       <c r="A5" s="9" t="s">
         <v>25</v>
       </c>
@@ -1363,7 +1984,7 @@
       <c r="N5" s="9"/>
       <c r="O5" s="16"/>
     </row>
-    <row r="6" spans="1:15" s="3" customFormat="1" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" s="19" customFormat="1" ht="31.5" spans="1:15">
       <c r="A6" s="9" t="s">
         <v>25</v>
       </c>
@@ -1396,7 +2017,7 @@
       <c r="N6" s="9"/>
       <c r="O6" s="16"/>
     </row>
-    <row r="7" spans="1:15" s="19" customFormat="1" ht="169.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" s="20" customFormat="1" ht="169.5" customHeight="1" spans="1:15">
       <c r="A7" s="9" t="s">
         <v>41</v>
       </c>
@@ -1421,7 +2042,7 @@
       <c r="N7" s="9"/>
       <c r="O7" s="9"/>
     </row>
-    <row r="8" spans="1:15" s="3" customFormat="1" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" s="19" customFormat="1" ht="31.5" spans="1:15">
       <c r="A8" s="9" t="s">
         <v>45</v>
       </c>
@@ -1452,7 +2073,7 @@
       <c r="N8" s="9"/>
       <c r="O8" s="16"/>
     </row>
-    <row r="9" spans="1:15" s="3" customFormat="1" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" s="19" customFormat="1" ht="31.5" spans="1:15">
       <c r="A9" s="9" t="s">
         <v>51</v>
       </c>
@@ -1470,7 +2091,7 @@
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
       <c r="I9" s="10"/>
-      <c r="J9" s="26"/>
+      <c r="J9" s="27"/>
       <c r="K9" s="9" t="s">
         <v>55</v>
       </c>
@@ -1481,7 +2102,7 @@
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
     </row>
-    <row r="10" spans="1:15" s="3" customFormat="1" ht="47" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" s="19" customFormat="1" ht="47.25" spans="1:15">
       <c r="A10" s="9" t="s">
         <v>56</v>
       </c>
@@ -1510,7 +2131,7 @@
       <c r="N10" s="9"/>
       <c r="O10" s="9"/>
     </row>
-    <row r="11" spans="1:15" s="19" customFormat="1" ht="62.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" s="20" customFormat="1" ht="63" spans="1:15">
       <c r="A11" s="9" t="s">
         <v>25</v>
       </c>
@@ -1539,7 +2160,7 @@
       <c r="N11" s="9"/>
       <c r="O11" s="9"/>
     </row>
-    <row r="12" spans="1:15" s="3" customFormat="1" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" s="19" customFormat="1" ht="31.5" spans="1:15">
       <c r="A12" s="9" t="s">
         <v>15</v>
       </c>
@@ -1574,7 +2195,7 @@
       <c r="N12" s="16"/>
       <c r="O12" s="16"/>
     </row>
-    <row r="13" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" s="19" customFormat="1" spans="1:15">
       <c r="A13" s="9" t="s">
         <v>71</v>
       </c>
@@ -1589,21 +2210,21 @@
         <v>74</v>
       </c>
       <c r="F13" s="11"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="26"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="27"/>
       <c r="K13" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="L13" s="24"/>
+      <c r="L13" s="25"/>
       <c r="M13" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="N13" s="24"/>
-      <c r="O13" s="24"/>
-    </row>
-    <row r="14" spans="1:15" s="3" customFormat="1" ht="47" x14ac:dyDescent="0.55000000000000004">
+      <c r="N13" s="25"/>
+      <c r="O13" s="25"/>
+    </row>
+    <row r="14" s="19" customFormat="1" ht="47.25" spans="1:15">
       <c r="A14" s="9" t="s">
         <v>75</v>
       </c>
@@ -1622,21 +2243,21 @@
       <c r="F14" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="26"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="27"/>
       <c r="K14" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="L14" s="24"/>
+      <c r="L14" s="25"/>
       <c r="M14" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="N14" s="24"/>
-      <c r="O14" s="24"/>
-    </row>
-    <row r="15" spans="1:15" s="3" customFormat="1" ht="31.35" x14ac:dyDescent="0.55000000000000004">
+      <c r="N14" s="25"/>
+      <c r="O14" s="25"/>
+    </row>
+    <row r="15" s="19" customFormat="1" ht="31.5" spans="1:15">
       <c r="A15" s="9" t="s">
         <v>75</v>
       </c>
@@ -1651,453 +2272,228 @@
         <v>83</v>
       </c>
       <c r="F15" s="11"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="26"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="27"/>
       <c r="K15" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="L15" s="24"/>
+      <c r="L15" s="25"/>
       <c r="M15" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="N15" s="24"/>
-      <c r="O15" s="24"/>
-    </row>
-    <row r="16" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="10"/>
+      <c r="N15" s="25"/>
+      <c r="O15" s="25"/>
+    </row>
+    <row r="16" s="19" customFormat="1" ht="78.75" spans="1:15">
+      <c r="A16" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>86</v>
+      </c>
       <c r="D16" s="10"/>
-      <c r="E16" s="11"/>
+      <c r="E16" s="11" t="s">
+        <v>87</v>
+      </c>
       <c r="F16" s="11"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="24"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="L16" s="25"/>
       <c r="M16" s="9"/>
-      <c r="N16" s="24"/>
-      <c r="O16" s="24"/>
-    </row>
-    <row r="17" spans="1:15" s="3" customFormat="1" ht="78.349999999999994" x14ac:dyDescent="0.55000000000000004">
+      <c r="N16" s="25"/>
+      <c r="O16" s="25"/>
+    </row>
+    <row r="17" s="19" customFormat="1" ht="78.75" spans="1:15">
       <c r="A17" s="9" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D17" s="10"/>
       <c r="E17" s="11" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="F17" s="11"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="26"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="27"/>
       <c r="K17" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="L17" s="24"/>
-      <c r="M17" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="N17" s="24"/>
-      <c r="O17" s="24"/>
-    </row>
-    <row r="18" spans="1:15" s="3" customFormat="1" ht="109.7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="9" t="s">
+      <c r="L17" s="25"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="25"/>
+      <c r="O17" s="25"/>
+    </row>
+    <row r="18" ht="31.5" spans="1:15">
+      <c r="A18" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="D18" s="24"/>
+      <c r="E18" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="F18" s="14"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="12"/>
+    </row>
+    <row r="19" ht="47.25" spans="1:15">
+      <c r="A19" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="D19" s="24"/>
+      <c r="E19" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="F19" s="14"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="D18" s="10"/>
-      <c r="E18" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="F18" s="11"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="27"/>
-      <c r="J18" s="26"/>
-      <c r="K18" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="L18" s="24"/>
-      <c r="M18" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="N18" s="24"/>
-      <c r="O18" s="24"/>
-    </row>
-    <row r="19" spans="1:15" s="3" customFormat="1" ht="78.349999999999994" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="F19" s="11"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
-      <c r="I19" s="27"/>
-      <c r="J19" s="26"/>
-      <c r="K19" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="L19" s="24"/>
-      <c r="M19" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="N19" s="24"/>
-      <c r="O19" s="24"/>
-    </row>
-    <row r="20" spans="1:15" s="3" customFormat="1" ht="109.7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="D20" s="10"/>
-      <c r="E20" s="11" t="s">
+      <c r="B20" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="F20" s="11"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
-      <c r="I20" s="27"/>
-      <c r="J20" s="26"/>
-      <c r="K20" s="9" t="s">
+      <c r="C20" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="L20" s="24"/>
-      <c r="M20" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="N20" s="24"/>
-      <c r="O20" s="24"/>
-    </row>
-    <row r="21" spans="1:15" s="3" customFormat="1" ht="78.349999999999994" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="B21" s="9" t="s">
+      <c r="D20" s="24"/>
+      <c r="E20" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="F20" s="14"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="25"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="D21" s="10"/>
-      <c r="E21" s="11" t="s">
+      <c r="B21" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="F21" s="11"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="24"/>
-      <c r="I21" s="27"/>
-      <c r="J21" s="26"/>
-      <c r="K21" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="L21" s="24"/>
-      <c r="M21" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="N21" s="24"/>
-      <c r="O21" s="24"/>
-    </row>
-    <row r="22" spans="1:15" s="3" customFormat="1" ht="109.7" x14ac:dyDescent="0.55000000000000004">
+      <c r="C21" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="D21" s="24"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="25"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
+    </row>
+    <row r="22" spans="1:15">
       <c r="A22" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="C22" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="D22" s="10"/>
-      <c r="E22" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="F22" s="11"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="27"/>
-      <c r="J22" s="26"/>
-      <c r="K22" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="L22" s="24"/>
-      <c r="M22" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="N22" s="24"/>
-      <c r="O22" s="24"/>
-    </row>
-    <row r="23" spans="1:15" s="3" customFormat="1" ht="31.35" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="B23" s="22" t="s">
-        <v>109</v>
-      </c>
-      <c r="C23" s="23" t="s">
-        <v>110</v>
-      </c>
-      <c r="D23" s="23"/>
-      <c r="E23" s="25" t="s">
-        <v>104</v>
-      </c>
-      <c r="F23" s="14"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="24"/>
-      <c r="I23" s="27"/>
-      <c r="J23" s="26"/>
-      <c r="K23" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="L23" s="24"/>
-      <c r="M23" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="N23" s="24"/>
-      <c r="O23" s="24"/>
-    </row>
-    <row r="24" spans="1:15" s="3" customFormat="1" ht="109.7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B24" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="C24" s="23" t="s">
-        <v>113</v>
-      </c>
-      <c r="D24" s="23"/>
-      <c r="E24" s="25" t="s">
-        <v>114</v>
-      </c>
-      <c r="F24" s="14"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="24"/>
-      <c r="I24" s="27"/>
-      <c r="J24" s="26"/>
-      <c r="K24" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="L24" s="24"/>
-      <c r="M24" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="N24" s="24"/>
-      <c r="O24" s="24"/>
-    </row>
-    <row r="25" spans="1:15" ht="31.35" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="B25" s="22" t="s">
-        <v>117</v>
-      </c>
-      <c r="C25" s="23" t="s">
-        <v>118</v>
-      </c>
-      <c r="D25" s="23" t="s">
-        <v>119</v>
-      </c>
-      <c r="E25" s="25" t="s">
-        <v>120</v>
-      </c>
-      <c r="F25" s="25" t="s">
-        <v>121</v>
-      </c>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="24" t="s">
-        <v>122</v>
-      </c>
-      <c r="L25" s="12"/>
-      <c r="M25" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="N25" s="12"/>
-      <c r="O25" s="12"/>
-    </row>
-    <row r="26" spans="1:15" ht="31.35" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="B26" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="C26" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="D26" s="23"/>
-      <c r="E26" s="25" t="s">
-        <v>125</v>
-      </c>
-      <c r="F26" s="14"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="14"/>
-      <c r="K26" s="24" t="s">
-        <v>126</v>
-      </c>
-      <c r="L26" s="12"/>
-      <c r="M26" s="12"/>
-      <c r="N26" s="12"/>
-      <c r="O26" s="12"/>
-    </row>
-    <row r="27" spans="1:15" ht="47" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="B27" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="C27" s="23" t="s">
-        <v>128</v>
-      </c>
-      <c r="D27" s="23"/>
-      <c r="E27" s="25" t="s">
-        <v>129</v>
-      </c>
-      <c r="F27" s="14"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="14"/>
-      <c r="K27" s="24" t="s">
-        <v>130</v>
-      </c>
-      <c r="L27" s="12"/>
-      <c r="M27" s="12"/>
-      <c r="N27" s="12"/>
-      <c r="O27" s="12"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="B28" s="22" t="s">
-        <v>131</v>
-      </c>
-      <c r="C28" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="D28" s="23"/>
-      <c r="E28" s="25" t="s">
-        <v>133</v>
-      </c>
-      <c r="F28" s="14"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="14"/>
-      <c r="K28" s="24"/>
-      <c r="L28" s="12"/>
-      <c r="M28" s="12"/>
-      <c r="N28" s="12"/>
-      <c r="O28" s="12"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="22" t="s">
-        <v>134</v>
-      </c>
-      <c r="B29" s="22" t="s">
-        <v>135</v>
-      </c>
-      <c r="C29" s="23" t="s">
-        <v>136</v>
-      </c>
-      <c r="D29" s="23"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="14"/>
-      <c r="K29" s="24"/>
-      <c r="L29" s="12"/>
-      <c r="M29" s="12"/>
-      <c r="N29" s="12"/>
-      <c r="O29" s="12"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="B30" s="22" t="s">
-        <v>138</v>
-      </c>
-      <c r="C30" s="23" t="s">
-        <v>136</v>
-      </c>
-      <c r="D30" s="23"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="13"/>
-      <c r="J30" s="14"/>
-      <c r="K30" s="24"/>
-      <c r="L30" s="12"/>
-      <c r="M30" s="12"/>
-      <c r="N30" s="12"/>
-      <c r="O30" s="12"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="25"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B28" sqref="B28"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A29" sqref="A29:A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.7" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="19.5" customWidth="1"/>
     <col min="2" max="2" width="39.5" style="6" customWidth="1"/>
     <col min="3" max="3" width="40" style="6" customWidth="1"/>
-    <col min="4" max="4" width="46.109375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="46.1066666666667" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4">
       <c r="A1" s="7" t="s">
-        <v>139</v>
+        <v>108</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -2109,435 +2505,522 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4">
       <c r="A2" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" s="5" customFormat="1" spans="1:4">
+      <c r="A6" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" s="5" customFormat="1" spans="1:4">
+      <c r="A7" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" s="5" customFormat="1" spans="1:4">
+      <c r="A8" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" s="5" customFormat="1" spans="1:4">
+      <c r="A9" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" s="5" customFormat="1" spans="1:4">
+      <c r="A10" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="11" s="5" customFormat="1" spans="1:4">
+      <c r="A11" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12" s="5" customFormat="1" spans="1:4">
+      <c r="A12" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="13" s="5" customFormat="1" spans="1:4">
+      <c r="A13" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="C13" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="D2" s="11" t="s">
+      <c r="D13" s="11" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="14" s="5" customFormat="1" spans="1:4">
+      <c r="A14" s="16" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B3" s="9" t="s">
+      <c r="B14" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="D3" s="11" t="s">
+      <c r="C14" s="17" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="9" t="s">
+      <c r="D14" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="B4" s="12" t="s">
+    </row>
+    <row r="15" s="5" customFormat="1" spans="1:4">
+      <c r="A15" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="B15" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="C4" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="B5" s="15" t="s">
+      <c r="C15" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="D15" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="D5" s="15" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="16" t="s">
+    </row>
+    <row r="16" s="5" customFormat="1" spans="1:4">
+      <c r="A16" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" s="5" customFormat="1" spans="1:4">
+      <c r="A17" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B17" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="C6" s="17" t="s">
-        <v>150</v>
-      </c>
-      <c r="D6" s="11" t="s">
+      <c r="C17" s="17" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="16" t="s">
+      <c r="D17" s="11" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="18" s="5" customFormat="1" spans="1:4">
+      <c r="A18" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="D7" s="11" t="s">
+      <c r="B18" s="9" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="16" t="s">
+      <c r="C18" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="D18" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="C8" s="17" t="s">
-        <v>155</v>
-      </c>
-      <c r="D8" s="11" t="s">
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="B19" s="9" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="B9" s="9" t="s">
+      <c r="C19" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="C9" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="D9" s="11" t="s">
+      <c r="D19" s="11" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="B10" s="9" t="s">
+    <row r="20" spans="1:4">
+      <c r="A20" s="16" t="s">
         <v>159</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="B20" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="16" t="s">
         <v>159</v>
       </c>
-      <c r="D10" s="11" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>161</v>
-      </c>
-      <c r="D11" s="11" t="s">
+      <c r="B21" s="9" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="B12" s="9" t="s">
+      <c r="C21" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="C12" s="17" t="s">
-        <v>163</v>
-      </c>
-      <c r="D12" s="11" t="s">
+      <c r="D21" s="11" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="B13" s="9" t="s">
+    <row r="22" spans="1:4">
+      <c r="A22" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="B22" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C22" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D22" s="11" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="16" t="s">
+    <row r="23" spans="1:4">
+      <c r="A23" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="B23" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="C23" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="C14" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="D14" s="11" t="s">
+      <c r="D23" s="11" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="16" t="s">
-        <v>168</v>
-      </c>
-      <c r="B15" s="9" t="s">
+    <row r="24" spans="1:4">
+      <c r="A24" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="B24" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="C15" s="17" t="s">
-        <v>171</v>
-      </c>
-      <c r="D15" s="11" t="s">
+      <c r="C24" s="10" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="16" t="s">
-        <v>168</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="16" t="s">
+      <c r="D24" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="B17" s="9" t="s">
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="B25" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C25" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="D25" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="D17" s="11" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="B18" s="9" t="s">
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="B26" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C26" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="D26" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="D18" s="11" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="B19" s="9" t="s">
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="18" t="s">
         <v>178</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="B27" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="18" t="s">
         <v>178</v>
       </c>
-      <c r="D19" s="11" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="16" t="s">
-        <v>180</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>181</v>
-      </c>
-      <c r="D20" s="11" t="s">
+      <c r="B28" s="6" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="16" t="s">
-        <v>180</v>
-      </c>
-      <c r="B21" s="9" t="s">
+      <c r="C28" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="C21" s="10" t="s">
-        <v>183</v>
-      </c>
-      <c r="D21" s="11" t="s">
+      <c r="D28" s="6" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="16" t="s">
-        <v>180</v>
-      </c>
-      <c r="B22" s="9" t="s">
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
         <v>185</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="B29" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
         <v>185</v>
       </c>
-      <c r="D22" s="11" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="16" t="s">
-        <v>180</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="16" t="s">
-        <v>180</v>
-      </c>
-      <c r="B24" s="9" t="s">
+      <c r="B30" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="C24" s="10" t="s">
-        <v>189</v>
-      </c>
-      <c r="D24" s="11" t="s">
+      <c r="C30" s="6" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="16" t="s">
-        <v>180</v>
-      </c>
-      <c r="B25" s="9" t="s">
+      <c r="D30" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="C25" s="10" t="s">
-        <v>191</v>
-      </c>
-      <c r="D25" s="11" t="s">
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>185</v>
+      </c>
+      <c r="B31" s="6" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="16" t="s">
-        <v>180</v>
-      </c>
-      <c r="B26" s="9" t="s">
+      <c r="C31" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="C26" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="D26" s="11" t="s">
+      <c r="D31" s="6" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="18" t="s">
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
+        <v>185</v>
+      </c>
+      <c r="B32" s="29" t="s">
         <v>195</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="C32" s="29" t="s">
+        <v>195</v>
+      </c>
+      <c r="D32" s="29" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>185</v>
+      </c>
+      <c r="B33" s="29" t="s">
         <v>196</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C33" s="29" t="s">
+        <v>196</v>
+      </c>
+      <c r="D33" s="29" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>185</v>
+      </c>
+      <c r="B34" s="29" t="s">
         <v>197</v>
       </c>
-      <c r="D27" s="6" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="18" t="s">
-        <v>195</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>201</v>
+      <c r="C34" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="D34" s="29" t="s">
+        <v>197</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.7" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="1" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="44.109375" customWidth="1"/>
-    <col min="2" max="2" width="32.109375" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" customWidth="1"/>
+    <col min="1" max="1" width="44.1066666666667" customWidth="1"/>
+    <col min="2" max="2" width="32.1066666666667" customWidth="1"/>
+    <col min="3" max="3" width="11.1066666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="2" ht="31.5" spans="1:4">
+      <c r="A2" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>203</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="28" t="s">
-        <v>208</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>206</v>
       </c>
       <c r="C2">
         <v>20200630</v>
       </c>
       <c r="D2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
tg: add possibility to add avillage field on the first form.
</commit_message>
<xml_diff>
--- a/SCH-STH/Impact assessments/Togo/tg_sch_sth_impact_2_child_202110.xlsx
+++ b/SCH-STH/Impact assessments/Togo/tg_sch_sth_impact_2_child_202110.xlsx
@@ -163,10 +163,10 @@
     <t>p_site</t>
   </si>
   <si>
-    <t>Select the site name</t>
-  </si>
-  <si>
-    <t>Sélectionner le nom de l'école</t>
+    <t>Select the village</t>
+  </si>
+  <si>
+    <t>Sélectionner le nom du village</t>
   </si>
   <si>
     <t>subdistrict_list= ${p_subdistrict}</t>
@@ -1932,10 +1932,10 @@
     <t>default_language</t>
   </si>
   <si>
-    <t>(Octobre 2021) - 2. SCH/STH – Enrôlement V3</t>
-  </si>
-  <si>
-    <t>tg_sch_sth_impact_2_child_202110_v3</t>
+    <t>(Octobre 2021) - 2. SCH/STH – Enrôlement V4</t>
+  </si>
+  <si>
+    <t>tg_sch_sth_impact_2_child_202110_v4</t>
   </si>
   <si>
     <t>French</t>
@@ -1946,10 +1946,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="30">
     <font>
@@ -1993,9 +1993,8 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -2008,15 +2007,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -2031,13 +2023,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -2046,17 +2031,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2069,24 +2045,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2107,8 +2067,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2123,6 +2106,14 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
@@ -2131,14 +2122,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2207,13 +2207,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2225,31 +2225,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2261,31 +2261,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2303,7 +2291,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2315,13 +2309,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2333,43 +2321,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2381,7 +2363,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2445,15 +2445,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -2465,6 +2456,50 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2483,186 +2518,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="34" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3080,7 +3080,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="$A3:$XFD3"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>

</xml_diff>